<commit_message>
Separate fits before and after sf helium transition
</commit_message>
<xml_diff>
--- a/May_June_sf_data.xlsx
+++ b/May_June_sf_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruthgregory/Documents/GitHub/Cooldown-Data-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6FEAA353-154D-D648-89D9-E5FD15F749DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DCC4742C-8C0D-1B49-A7C8-59066979C150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="500" windowWidth="37180" windowHeight="19380"/>
+    <workbookView xWindow="28920" yWindow="500" windowWidth="37180" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sf_data" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4005,11 +4005,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="AB42" sqref="AB42"/>
+    <sheetView tabSelected="1" topLeftCell="K28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4414,23 +4414,23 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
-        <f t="shared" ref="B17:B23" si="0">B5-B4</f>
+        <f t="shared" ref="B17:B22" si="0">B5-B4</f>
         <v>1.5179372747825013E-9</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ref="E17:E25" si="1">E5-E4</f>
+        <f>E5-E4</f>
         <v>9.8203638959690031E-10</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17:H23" si="2">H5-H4</f>
+        <f t="shared" ref="H17:H22" si="1">H5-H4</f>
         <v>2.8920112811506009E-9</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" ref="K17:K23" si="3">K5-K4</f>
+        <f t="shared" ref="K17:K22" si="2">K5-K4</f>
         <v>3.1898744199668997E-9</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" ref="N17:N23" si="4">N5-N4</f>
+        <f t="shared" ref="N17:N22" si="3">N5-N4</f>
         <v>3.294108077056001E-9</v>
       </c>
     </row>
@@ -4440,19 +4440,19 @@
         <v>6.2909657091439694E-10</v>
       </c>
       <c r="E18" s="1">
+        <f t="shared" ref="E17:E24" si="4">E6-E5</f>
+        <v>9.7266865668419765E-10</v>
+      </c>
+      <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>9.7266865668419765E-10</v>
-      </c>
-      <c r="H18" s="1">
+        <v>2.9785321842500009E-9</v>
+      </c>
+      <c r="K18" s="1">
         <f t="shared" si="2"/>
-        <v>2.9785321842500009E-9</v>
-      </c>
-      <c r="K18" s="1">
+        <v>3.9259197708737985E-9</v>
+      </c>
+      <c r="N18" s="1">
         <f t="shared" si="3"/>
-        <v>3.9259197708737985E-9</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="4"/>
         <v>3.0653828724313003E-9</v>
       </c>
     </row>
@@ -4462,19 +4462,19 @@
         <v>2.7327390550849827E-10</v>
       </c>
       <c r="E19" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1651619072356014E-9</v>
+      </c>
+      <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>1.1651619072356014E-9</v>
-      </c>
-      <c r="H19" s="1">
+        <v>2.7743340041897983E-9</v>
+      </c>
+      <c r="K19" s="1">
         <f t="shared" si="2"/>
-        <v>2.7743340041897983E-9</v>
-      </c>
-      <c r="K19" s="1">
+        <v>4.0275204756274036E-9</v>
+      </c>
+      <c r="N19" s="1">
         <f t="shared" si="3"/>
-        <v>4.0275204756274036E-9</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="4"/>
         <v>2.1731381815034971E-9</v>
       </c>
     </row>
@@ -4484,19 +4484,19 @@
         <v>4.5051919223049844E-10</v>
       </c>
       <c r="E20" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5400359153016989E-9</v>
+      </c>
+      <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>1.5400359153016989E-9</v>
-      </c>
-      <c r="H20" s="1">
+        <v>2.3037426085923015E-9</v>
+      </c>
+      <c r="K20" s="1">
         <f t="shared" si="2"/>
-        <v>2.3037426085923015E-9</v>
-      </c>
-      <c r="K20" s="1">
+        <v>3.4468299517224007E-9</v>
+      </c>
+      <c r="N20" s="1">
         <f t="shared" si="3"/>
-        <v>3.4468299517224007E-9</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="4"/>
         <v>5.0864342931470215E-10</v>
       </c>
     </row>
@@ -4506,19 +4506,19 @@
         <v>1.133160877926501E-9</v>
       </c>
       <c r="E21" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0234481645878007E-9</v>
+      </c>
+      <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>2.0234481645878007E-9</v>
-      </c>
-      <c r="H21" s="1">
+        <v>1.5600830168138013E-9</v>
+      </c>
+      <c r="K21" s="1">
         <f t="shared" si="2"/>
-        <v>1.5600830168138013E-9</v>
-      </c>
-      <c r="K21" s="1">
+        <v>2.2171262405658006E-9</v>
+      </c>
+      <c r="N21" s="1">
         <f t="shared" si="3"/>
-        <v>2.2171262405658006E-9</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" si="4"/>
         <v>-2.1257266287578977E-9</v>
       </c>
     </row>
@@ -4528,19 +4528,19 @@
         <v>2.3680874601396005E-9</v>
       </c>
       <c r="E22" s="1">
+        <f t="shared" si="4"/>
+        <v>2.6841017361061992E-9</v>
+      </c>
+      <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>2.6841017361061992E-9</v>
-      </c>
-      <c r="H22" s="1">
+        <v>5.2612092897259789E-10</v>
+      </c>
+      <c r="K22" s="1">
         <f t="shared" si="2"/>
-        <v>5.2612092897259789E-10</v>
-      </c>
-      <c r="K22" s="1">
+        <v>3.3274977218229656E-10</v>
+      </c>
+      <c r="N22" s="1">
         <f t="shared" si="3"/>
-        <v>3.3274977218229656E-10</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="4"/>
         <v>-4.9007208959205014E-9</v>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
         <v>4.0925540061573E-9</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.648232425905201E-9</v>
       </c>
       <c r="H23" s="1">
@@ -4572,7 +4572,7 @@
         <v>6.3906281909318023E-9</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.9969097014699317E-11</v>
       </c>
     </row>

</xml_diff>